<commit_message>
Fixing Maxime_Eeraerts management categories
Conventional -> conventional
</commit_message>
<xml_diff>
--- a/Processing_files/Datasets_Processing/Templates processed automatically/Maxime_Eeraerts_Prunus_avium_Belgium_2017_2019_REV.xlsx
+++ b/Processing_files/Datasets_Processing/Templates processed automatically/Maxime_Eeraerts_Prunus_avium_Belgium_2017_2019_REV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -842,7 +842,7 @@
     <t xml:space="preserve">Kordia and Regina</t>
   </si>
   <si>
-    <t xml:space="preserve">Conventional</t>
+    <t xml:space="preserve">conventional</t>
   </si>
   <si>
     <t xml:space="preserve">Belgium</t>
@@ -1727,15 +1727,15 @@
   <dimension ref="A1:BL115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+      <selection pane="topLeft" activeCell="C54" activeCellId="1" sqref="E2:E26 C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="37.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="138.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="3" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="3" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,10 +3565,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C44" activeCellId="1" sqref="E2:E26 C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="17.9"/>
@@ -3576,15 +3576,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="22.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="45" width="15.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="45" width="12.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="45" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="45" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="45" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="45" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="45" width="82.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="45" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="45" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="45" width="12.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="45" width="12.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="15" style="45" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="15" style="45" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" s="51" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9210,11 +9210,11 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="E2:E26 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.69"/>
@@ -9302,18 +9302,18 @@
   </sheetPr>
   <dimension ref="A1:BM26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="17.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="46" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="46" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="46" width="12.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="46" width="16.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="46" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="46" width="11"/>
@@ -9326,7 +9326,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="46" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="46" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="20" style="46" width="14.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="46" width="11.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="46" width="10.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="46" width="10.5"/>
@@ -9337,27 +9337,27 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="46" width="30.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="46" width="18.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="46" width="20.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="46" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="46" width="11.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="46" width="11.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="38" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="38" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="46" width="11.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="46" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="46" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="46" width="14.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="43" min="43" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="43" min="43" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="46" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="46" width="11.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="46" min="46" style="46" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="46" min="46" style="46" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="46" width="17.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="46" width="16.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="46" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="46" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="46" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="46" width="13.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="46" width="13.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="46" width="14.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="46" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="46" width="15.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="46" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="46" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="46" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="46" width="14.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="46" width="12.7"/>
@@ -9366,8 +9366,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="46" width="38.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="46" width="22.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="52" width="48.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="78" min="66" style="46" width="10.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="79" style="45" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="78" min="66" style="46" width="10.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="79" style="45" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" s="70" customFormat="true" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12089,10 +12089,10 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="E2:E26 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.4"/>

</xml_diff>

<commit_message>
Fix the guild of Eupeodes luniger in Maxime_Eeraerts_Prunus_avium_Belgium_2017_2019
</commit_message>
<xml_diff>
--- a/Processing_files/Datasets_Processing/Templates processed automatically/Maxime_Eeraerts_Prunus_avium_Belgium_2017_2019_REV.xlsx
+++ b/Processing_files/Datasets_Processing/Templates processed automatically/Maxime_Eeraerts_Prunus_avium_Belgium_2017_2019_REV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:BL115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="1" sqref="Q2:Q26 C54"/>
+      <selection pane="topLeft" activeCell="C54" activeCellId="1" sqref="F56 C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3562,13 +3562,13 @@
   </sheetPr>
   <dimension ref="A1:N160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C44" activeCellId="1" sqref="Q2:Q26 C44"/>
+      <selection pane="bottomLeft" activeCell="D56" activeCellId="1" sqref="F56 D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="17.9"/>
@@ -5534,7 +5534,7 @@
         <v>186</v>
       </c>
       <c r="F56" s="45" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="G56" s="46" t="n">
         <v>1</v>
@@ -9211,7 +9211,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="Q2:Q26 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="F56 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9302,11 +9302,11 @@
   </sheetPr>
   <dimension ref="A1:BM26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2:Q26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="F56 Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="17.9"/>
@@ -12089,7 +12089,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="Q2:Q26 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="F56 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>